<commit_message>
Manually change users and multiple excel writes
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\ExcelDriveSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HobbyProjects\DriveAssistant\ExcelDriveSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B26D64-5F91-483D-B4A8-43E2642CE970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4779A110-B272-497F-B19E-F962B31AF645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="30105" yWindow="780" windowWidth="17220" windowHeight="8850" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="4" r:id="rId1"/>
@@ -706,29 +706,29 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
-    <col min="9" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="6" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="6" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="12" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="6"/>
+    <col min="15" max="15" width="8.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
         <v>Drive Summary Stefan August 2024</v>
@@ -739,7 +739,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -747,7 +747,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -778,7 +778,7 @@
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -789,10 +789,10 @@
         <v>24</v>
       </c>
       <c r="F6" s="23">
-        <v>611.47199999999998</v>
+        <v>828</v>
       </c>
       <c r="G6" s="16">
-        <v>342</v>
+        <v>542</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>19</v>
@@ -816,12 +816,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="16">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
@@ -829,11 +829,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>2707.9474285714286</v>
+        <v>2333.454545454545</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1514.5714285714284</v>
+        <v>1527.4545454545455</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -857,13 +857,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -889,7 +889,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -928,24 +928,24 @@
       </c>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2620</v>
+        <v>2556</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>87.353142857142856</v>
+        <v>75.272727272727266</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>48.857142857142854</v>
+        <v>49.272727272727273</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -969,7 +969,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="I11" s="1">
         <v>600</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1031,11 +1031,11 @@
       </c>
       <c r="F13" s="18">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
-        <v>137.52800000000002</v>
+        <v>71</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1053,7 +1053,7 @@
       <c r="O13"/>
       <c r="P13"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="Q14"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15" s="11"/>
       <c r="I15" s="1">
         <v>1200</v>
@@ -1094,7 +1094,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
         <v>30</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -1162,7 +1162,7 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -1184,7 +1184,7 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -1205,7 +1205,7 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -1224,13 +1224,13 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -1238,133 +1238,133 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="14"/>
       <c r="P24"/>
       <c r="Q24"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25" s="14"/>
       <c r="P25"/>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M27" s="6"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M28" s="6"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="J29" s="4"/>
       <c r="M29" s="6"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="20"/>
       <c r="M31" s="6"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E32" s="19"/>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="M32" s="6"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E33" s="19"/>
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
       <c r="M33" s="6"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E34" s="19"/>
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
       <c r="K34" s="3"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E35" s="19"/>
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E36" s="19"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E37" s="19"/>
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E38" s="19"/>
       <c r="F38" s="21"/>
       <c r="G38" s="20"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E39" s="19"/>
       <c r="F39" s="21"/>
       <c r="G39" s="22"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="H41" s="13"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42" s="13"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I44" s="3"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M50" s="6"/>
     </row>
   </sheetData>
@@ -1388,29 +1388,29 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:N13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
-    <col min="9" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="6" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="6" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="12" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="6"/>
+    <col min="15" max="15" width="8.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
         <v>Drive Summary Christiaan August 2024</v>
@@ -1421,7 +1421,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -1429,7 +1429,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1471,10 +1471,10 @@
         <v>24</v>
       </c>
       <c r="F6" s="23">
-        <v>292.83300000000003</v>
+        <v>407</v>
       </c>
       <c r="G6" s="16">
-        <v>347</v>
+        <v>547</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>19</v>
@@ -1498,12 +1498,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="16">
-        <v>124</v>
+        <v>188</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
@@ -1511,11 +1511,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1296.8318571428572</v>
+        <v>1147</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1536.7142857142856</v>
+        <v>1541.5454545454545</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1539,13 +1539,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -1571,7 +1571,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1610,24 +1610,24 @@
       </c>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2354</v>
+        <v>2398</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>41.833285714285715</v>
+        <v>37</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.571428571428569</v>
+        <v>49.727272727272727</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1651,7 +1651,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="I11" s="1">
         <v>600</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1713,11 +1713,11 @@
       </c>
       <c r="F13" s="18">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
-        <v>6.1669999999999732</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1735,7 +1735,7 @@
       <c r="O13"/>
       <c r="P13"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="Q14"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15" s="11"/>
       <c r="I15" s="1">
         <v>1200</v>
@@ -1776,7 +1776,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1798,7 +1798,7 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
         <v>30</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -1844,7 +1844,7 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -1866,7 +1866,7 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -1887,7 +1887,7 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -1906,13 +1906,13 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -1920,133 +1920,133 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="14"/>
       <c r="P24"/>
       <c r="Q24"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25" s="14"/>
       <c r="P25"/>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M27" s="6"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M28" s="6"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="J29" s="4"/>
       <c r="M29" s="6"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="20"/>
       <c r="M31" s="6"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E32" s="19"/>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="M32" s="6"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E33" s="19"/>
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
       <c r="M33" s="6"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E34" s="19"/>
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
       <c r="K34" s="3"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E35" s="19"/>
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E36" s="19"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E37" s="19"/>
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E38" s="19"/>
       <c r="F38" s="21"/>
       <c r="G38" s="20"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E39" s="19"/>
       <c r="F39" s="21"/>
       <c r="G39" s="22"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="H41" s="13"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42" s="13"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I44" s="3"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M50" s="6"/>
     </row>
   </sheetData>
@@ -2073,26 +2073,26 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
-    <col min="9" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="6" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="6" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="12" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="6"/>
+    <col min="15" max="15" width="8.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
         <v>Drive Summary Derrick August 2024</v>
@@ -2103,7 +2103,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2111,13 +2111,13 @@
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="18">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
@@ -2142,16 +2142,22 @@
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="16">
+        <v>150</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="23">
+        <v>316</v>
+      </c>
+      <c r="G6" s="16">
+        <v>548</v>
+      </c>
       <c r="I6" s="7" t="s">
         <v>19</v>
       </c>
@@ -2174,22 +2180,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="16">
+        <v>300</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>890.5454545454545</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>1544.3636363636365</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2213,13 +2221,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -2245,11 +2253,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="16">
+        <v>300</v>
+      </c>
       <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
@@ -2282,24 +2292,24 @@
       </c>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>1500</v>
+        <v>2510</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>28.727272727272727</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>49.81818181818182</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -2323,7 +2333,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="I11" s="1">
         <v>600</v>
       </c>
@@ -2346,13 +2356,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
-        <v>Bronze</v>
+        <v>Diamond</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="19"/>
@@ -2373,21 +2383,23 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="16">
+        <v>1179.26</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="18">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2405,13 +2417,13 @@
       <c r="O13"/>
       <c r="P13"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>0</v>
+        <v>5896.3</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>
@@ -2429,7 +2441,7 @@
       <c r="Q14"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D15" s="11"/>
       <c r="I15" s="1">
         <v>1200</v>
@@ -2446,7 +2458,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -2468,7 +2480,7 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
         <v>30</v>
       </c>
@@ -2492,7 +2504,7 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -2514,7 +2526,7 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -2536,7 +2548,7 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -2557,7 +2569,7 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -2576,13 +2588,13 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -2590,133 +2602,133 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="14"/>
       <c r="P24"/>
       <c r="Q24"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25" s="14"/>
       <c r="P25"/>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M27" s="6"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M28" s="6"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="J29" s="4"/>
       <c r="M29" s="6"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="20"/>
       <c r="M31" s="6"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E32" s="19"/>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="M32" s="6"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E33" s="19"/>
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
       <c r="M33" s="6"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E34" s="19"/>
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
       <c r="K34" s="3"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E35" s="19"/>
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E36" s="19"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E37" s="19"/>
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E38" s="19"/>
       <c r="F38" s="21"/>
       <c r="G38" s="20"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E39" s="19"/>
       <c r="F39" s="21"/>
       <c r="G39" s="22"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="H41" s="13"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42" s="13"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I44" s="3"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M50" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Single excel write for all users
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HobbyProjects\DriveAssistant\ExcelDriveSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4779A110-B272-497F-B19E-F962B31AF645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74914D69-4F10-431D-A37A-8975B7D92984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="780" windowWidth="17220" windowHeight="8850" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="4" r:id="rId1"/>
@@ -706,7 +706,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,8 +1387,8 @@
   </sheetPr>
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,7 +1471,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="23">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="G6" s="16">
         <v>547</v>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1147</v>
+        <v>1155.4545454545455</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>37</v>
+        <v>37.272727272727273</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="F13" s="18">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
@@ -2069,8 +2069,8 @@
   </sheetPr>
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Excel remaining field added
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\ExcelDriveSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DA425B-E848-4C31-B87F-4D5FE1FF2A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F4C76A-A7D2-4791-886E-C7FE4AF1DD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="36">
   <si>
     <t>End</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Derrick</t>
+  </si>
+  <si>
+    <t>Remaining</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,6 +370,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1388,7 +1394,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2076,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:P1048576"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,6 +2431,10 @@
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
         <v>5896.3</v>
       </c>
+      <c r="E14" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="I14" s="1">
         <v>1050</v>
       </c>

</xml_diff>

<commit_message>
Multiple email receivers added in bcc
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\ExcelDriveSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBC302A-4B60-44F7-A785-6F1F9D92BCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A6E2CF-8AE0-4D76-82F6-364469264038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="4" r:id="rId1"/>
@@ -703,7 +703,7 @@
   <dimension ref="B2:V50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="C5" s="18">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
@@ -785,10 +785,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="23">
-        <v>1057</v>
+        <v>1097</v>
       </c>
       <c r="G6" s="16">
-        <v>642</v>
+        <v>856</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
@@ -820,7 +820,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="16">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
@@ -828,11 +828,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>2340.5</v>
+        <v>1889.2777777777778</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1421.5714285714284</v>
+        <v>1474.2222222222222</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -934,18 +934,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2508</v>
+        <v>2549</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>75.5</v>
+        <v>60.944444444444443</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>45.857142857142854</v>
+        <v>47.555555555555557</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1033,11 +1033,11 @@
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>142</v>
+        <v>401</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>850</v>
+        <v>650</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1398,8 +1398,8 @@
   </sheetPr>
   <dimension ref="B2:V50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,10 +1481,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="23">
-        <v>626</v>
+        <v>817</v>
       </c>
       <c r="G6" s="16">
-        <v>697</v>
+        <v>895</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
@@ -1516,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="16">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
@@ -1524,11 +1524,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1386.1428571428571</v>
+        <v>1407.0555555555554</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1543.3571428571429</v>
+        <v>1541.3888888888889</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -1630,18 +1630,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2358</v>
+        <v>2384</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>44.714285714285715</v>
+        <v>45.388888888888886</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.785714285714285</v>
+        <v>49.722222222222221</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1722,18 +1722,18 @@
         <v>1</v>
       </c>
       <c r="C13" s="27">
-        <v>848.71</v>
+        <v>1048.71</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>1172</v>
+        <v>1431</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>850</v>
+        <v>650</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>2970.4849999999997</v>
+        <v>3670.4849999999997</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>
@@ -2094,8 +2094,8 @@
   </sheetPr>
   <dimension ref="B2:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,10 +2177,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="23">
-        <v>368</v>
+        <v>490</v>
       </c>
       <c r="G6" s="16">
-        <v>698</v>
+        <v>890</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
@@ -2220,11 +2220,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>814.85714285714278</v>
+        <v>843.88888888888891</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1545.5714285714284</v>
+        <v>1532.7777777777778</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -2326,18 +2326,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2510</v>
+        <v>2490</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>26.285714285714285</v>
+        <v>27.222222222222221</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.857142857142854</v>
+        <v>49.444444444444443</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
-        <v>Diamond</v>
+        <v>Gold</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="19"/>
@@ -2425,11 +2425,11 @@
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>81</v>
+        <v>2208</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>850</v>
+        <v>650</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>5896.3</v>
+        <v>4127.41</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>

</xml_diff>

<commit_message>
Excel template checkbox removed
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\ExcelDriveSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A6E2CF-8AE0-4D76-82F6-364469264038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E499392B-501C-4B65-8E7E-88D09C8AE449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="4" r:id="rId1"/>
@@ -702,8 +702,8 @@
   </sheetPr>
   <dimension ref="B2:V50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,10 +785,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="23">
-        <v>1097</v>
+        <v>1189</v>
       </c>
       <c r="G6" s="16">
-        <v>856</v>
+        <v>1006</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
@@ -820,7 +820,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="16">
-        <v>289</v>
+        <v>256</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
@@ -828,11 +828,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1889.2777777777778</v>
+        <v>1755.1904761904761</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1474.2222222222222</v>
+        <v>1485.047619047619</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -934,18 +934,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2549</v>
+        <v>2516</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>60.944444444444443</v>
+        <v>56.61904761904762</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>47.555555555555557</v>
+        <v>47.904761904761905</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1033,11 +1033,11 @@
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>401</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1481,10 +1481,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="23">
-        <v>817</v>
+        <v>1068</v>
       </c>
       <c r="G6" s="16">
-        <v>895</v>
+        <v>1042</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
@@ -1516,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="16">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
@@ -1524,11 +1524,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1407.0555555555554</v>
+        <v>1576.5714285714284</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1541.3888888888889</v>
+        <v>1538.1904761904761</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -1630,18 +1630,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2384</v>
+        <v>2296</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>45.388888888888886</v>
+        <v>50.857142857142854</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.722222222222221</v>
+        <v>49.61904761904762</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1729,11 +1729,11 @@
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>1431</v>
+        <v>730</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2177,10 +2177,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="23">
-        <v>490</v>
+        <v>533</v>
       </c>
       <c r="G6" s="16">
-        <v>890</v>
+        <v>1040</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>17</v>
@@ -2220,11 +2220,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>843.88888888888891</v>
+        <v>786.80952380952374</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1532.7777777777778</v>
+        <v>1535.2380952380952</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2333,11 +2333,11 @@
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>27.222222222222221</v>
+        <v>25.38095238095238</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.444444444444443</v>
+        <v>49.523809523809526</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -2425,11 +2425,11 @@
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>2208</v>
+        <v>2165</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>

</xml_diff>

<commit_message>
Cache speedlimit data and store api responses
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveAssistant/ExcelDriveSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{E499392B-501C-4B65-8E7E-88D09C8AE449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D6990F9-9019-44B2-A1FD-BF15DD93E760}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{E499392B-501C-4B65-8E7E-88D09C8AE449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B22BDF46-4336-4E8B-8A1E-5F780806FEB9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="4" r:id="rId1"/>
@@ -38,103 +38,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="34">
+  <si>
+    <t>Driving Profile</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Distance Brackets</t>
+  </si>
+  <si>
+    <t>Driving Status</t>
+  </si>
+  <si>
+    <t>Night Time drive</t>
+  </si>
+  <si>
+    <t>Claim Free Years</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Fuel %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Night Time Driving</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Distance Points</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>MultiPoint Check</t>
+  </si>
+  <si>
+    <t>Daily Average</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Accumulated Points</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>Vitality Drive Status</t>
+  </si>
+  <si>
+    <t>Qualifying Fuel Spend</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
   <si>
     <t>Fuel Cash Back in Miles</t>
   </si>
   <si>
-    <t>Qualifying Fuel Spend</t>
-  </si>
-  <si>
-    <t>Vitality Drive Status</t>
-  </si>
-  <si>
-    <t>Diamond</t>
-  </si>
-  <si>
-    <t>Accumulated Points</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>MultiPoint Check</t>
-  </si>
-  <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>Distance Points</t>
-  </si>
-  <si>
-    <t>Bronze</t>
-  </si>
-  <si>
-    <t>Night Time Driving</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Claim Free Years</t>
-  </si>
-  <si>
-    <t>Fuel %</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>Upper</t>
-  </si>
-  <si>
-    <t>Lower</t>
-  </si>
-  <si>
-    <t>Driving Profile</t>
-  </si>
-  <si>
-    <t>Distance</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
-  <si>
     <t>Predict Status</t>
-  </si>
-  <si>
-    <t>Prediction</t>
-  </si>
-  <si>
-    <t>Remaining</t>
-  </si>
-  <si>
-    <t>Distance Brackets</t>
-  </si>
-  <si>
-    <t>Driving Status</t>
-  </si>
-  <si>
-    <t>Daily Average</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
-    <t>Christiaan</t>
-  </si>
-  <si>
-    <t>Derrick</t>
-  </si>
-  <si>
-    <t>Stefan</t>
   </si>
   <si>
     <t>The predicted status gives a more realistic prediction of the driving status. 
 If the prediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket.</t>
+  </si>
+  <si>
+    <t>Christiaan</t>
+  </si>
+  <si>
+    <t>Derrick</t>
   </si>
 </sst>
 </file>
@@ -267,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,6 +370,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -706,8 +715,8 @@
   </sheetPr>
   <dimension ref="B2:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +738,7 @@
     <row r="2" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", N13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan September 2024</v>
+        <v>Drive Summary Stefan October 2024</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
@@ -747,73 +756,83 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C5" s="18">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>September 2024</v>
+        <v>October 2024</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="J5" s="30"/>
       <c r="K5" s="31"/>
       <c r="M5" s="29" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="31"/>
+      <c r="R5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="34"/>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="16">
         <v>300</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F6" s="23">
-        <v>529</v>
+        <v>759</v>
       </c>
       <c r="G6" s="16">
-        <v>742</v>
+        <v>973</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="T6"/>
       <c r="U6" s="26"/>
@@ -821,23 +840,22 @@
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="16">
-        <f>300-24</f>
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1058</v>
+        <v>1176.45</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1484</v>
+        <v>1508.1499999999999</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -855,20 +873,27 @@
         <v>799</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="P7" s="10">
         <v>0.05</v>
       </c>
+      <c r="R7" s="6">
+        <v>10</v>
+      </c>
+      <c r="S7" s="6">
+        <f>R7*2</f>
+        <v>20</v>
+      </c>
       <c r="U7" s="9"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -888,27 +913,34 @@
         <v>1599</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="P8" s="10">
         <v>0.1</v>
       </c>
+      <c r="R8" s="6">
+        <v>2</v>
+      </c>
+      <c r="S8" s="6">
+        <f>R8*2</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C9" s="16">
         <v>300</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1">
         <v>300</v>
@@ -926,7 +958,7 @@
         <v>2199</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="P9" s="10">
         <v>0.2</v>
@@ -935,22 +967,22 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2608</v>
+        <v>2600</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>35.266666666666666</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.466666666666669</v>
+        <v>48.65</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -968,7 +1000,7 @@
         <v>2499</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="P10" s="10">
         <v>0.35</v>
@@ -991,7 +1023,7 @@
         <v>3000</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P11" s="10">
         <v>0.5</v>
@@ -1000,7 +1032,7 @@
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
@@ -1009,10 +1041,10 @@
       <c r="D12" s="9"/>
       <c r="E12" s="19"/>
       <c r="F12" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1">
         <v>750</v>
@@ -1028,21 +1060,21 @@
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C13" s="27">
-        <v>1515</v>
+        <v>1697.23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>819</v>
+        <v>889</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>750</v>
+        <v>550</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1057,7 +1089,7 @@
         <v>27</v>
       </c>
       <c r="N13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P13"/>
       <c r="S13" s="26"/>
@@ -1065,11 +1097,11 @@
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>7575</v>
+        <v>8486.15</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>
@@ -1107,7 +1139,7 @@
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C16" s="24" t="b">
         <v>0</v>
@@ -1385,14 +1417,15 @@
   <protectedRanges>
     <protectedRange sqref="F6:G6 C6:C7 C9 C13 C16" name="RequiresInput"/>
   </protectedRanges>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="B17:G19"/>
     <mergeCell ref="I5:K5"/>
+    <mergeCell ref="R5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1403,8 +1436,8 @@
   </sheetPr>
   <dimension ref="B2:V50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1459,7 @@
     <row r="2" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", N13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Christiaan September 2024</v>
+        <v>Drive Summary Christiaan October 2024</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
@@ -1444,73 +1477,83 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C5" s="18">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>1497</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>September 2024</v>
+        <v>October 2024</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="J5" s="30"/>
       <c r="K5" s="31"/>
       <c r="M5" s="29" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="31"/>
+      <c r="R5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="34"/>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="16">
         <v>150</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F6" s="23">
-        <v>1432</v>
+        <v>1546</v>
       </c>
       <c r="G6" s="16">
-        <v>747</v>
+        <v>984</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="T6"/>
       <c r="U6" s="26"/>
@@ -1518,22 +1561,22 @@
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="16">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>2864</v>
+        <v>2396.2999999999997</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1494</v>
+        <v>1525.2</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1551,20 +1594,27 @@
         <v>799</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="P7" s="10">
         <v>0.05</v>
       </c>
+      <c r="R7" s="6">
+        <v>25</v>
+      </c>
+      <c r="S7" s="6">
+        <f>R7*2</f>
+        <v>50</v>
+      </c>
       <c r="U7" s="9"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -1584,7 +1634,7 @@
         <v>1599</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="P8" s="10">
         <v>0.1</v>
@@ -1592,19 +1642,19 @@
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C9" s="16">
         <v>300</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1">
         <v>300</v>
@@ -1622,7 +1672,7 @@
         <v>2199</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="P9" s="10">
         <v>0.2</v>
@@ -1631,22 +1681,22 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2317</v>
+        <v>2350</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>95.466666666666669</v>
+        <v>77.3</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.8</v>
+        <v>49.2</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1664,7 +1714,7 @@
         <v>2499</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="P10" s="10">
         <v>0.35</v>
@@ -1687,7 +1737,7 @@
         <v>3000</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P11" s="10">
         <v>0.5</v>
@@ -1696,7 +1746,7 @@
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
@@ -1705,10 +1755,10 @@
       <c r="D12" s="9"/>
       <c r="E12" s="19"/>
       <c r="F12" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1">
         <v>750</v>
@@ -1724,21 +1774,21 @@
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C13" s="27">
-        <v>791.03</v>
+        <v>1402.06</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>816</v>
+        <v>1152</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>750</v>
+        <v>550</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1753,7 +1803,7 @@
         <v>27</v>
       </c>
       <c r="N13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="P13"/>
       <c r="S13" s="26"/>
@@ -1761,11 +1811,11 @@
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>2768.6049999999996</v>
+        <v>4907.2099999999991</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>
@@ -1803,7 +1853,7 @@
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C16" s="24" t="b">
         <v>0</v>
@@ -2081,14 +2131,15 @@
   <protectedRanges>
     <protectedRange sqref="F6:G6 C6:C7 C9 C13 C16" name="RequiresInput"/>
   </protectedRanges>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="B17:G19"/>
+    <mergeCell ref="R5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2100,7 +2151,7 @@
   <dimension ref="B2:V50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,7 +2173,7 @@
     <row r="2" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", N13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Derrick September 2024</v>
+        <v>Drive Summary Derrick October 2024</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
@@ -2140,30 +2191,30 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C5" s="18">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>1466</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>September 2024</v>
+        <v>October 2024</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="J5" s="30"/>
       <c r="K5" s="31"/>
       <c r="M5" s="29" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
@@ -2173,40 +2224,40 @@
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="16">
         <v>150</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F6" s="23">
-        <v>703</v>
+        <v>415</v>
       </c>
       <c r="G6" s="16">
-        <v>716</v>
+        <v>992</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="T6"/>
       <c r="U6" s="26"/>
@@ -2214,22 +2265,22 @@
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="16">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1406</v>
+        <v>643.25</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1432</v>
+        <v>1537.6000000000001</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2247,7 +2298,7 @@
         <v>799</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="P7" s="10">
         <v>0.05</v>
@@ -2256,11 +2307,11 @@
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -2280,7 +2331,7 @@
         <v>1599</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="P8" s="10">
         <v>0.1</v>
@@ -2288,19 +2339,19 @@
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C9" s="16">
         <v>300</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1">
         <v>300</v>
@@ -2318,7 +2369,7 @@
         <v>2199</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="P9" s="10">
         <v>0.2</v>
@@ -2327,22 +2378,22 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2436</v>
+        <v>2478</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>46.866666666666667</v>
+        <v>20.75</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>47.733333333333334</v>
+        <v>49.6</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -2360,7 +2411,7 @@
         <v>2499</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="P10" s="10">
         <v>0.35</v>
@@ -2383,7 +2434,7 @@
         <v>3000</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P11" s="10">
         <v>0.5</v>
@@ -2392,7 +2443,7 @@
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
@@ -2401,10 +2452,10 @@
       <c r="D12" s="9"/>
       <c r="E12" s="19"/>
       <c r="F12" s="7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1">
         <v>750</v>
@@ -2420,21 +2471,21 @@
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C13" s="27">
-        <v>1341.73</v>
+        <v>822</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" s="18">
         <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
-        <v>1695</v>
+        <v>1983</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>750</v>
+        <v>550</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2449,7 +2500,7 @@
         <v>27</v>
       </c>
       <c r="N13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="P13"/>
       <c r="S13" s="26"/>
@@ -2457,11 +2508,11 @@
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>4696.0549999999994</v>
+        <v>2877</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>
@@ -2499,7 +2550,7 @@
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C16" s="24" t="b">
         <v>0</v>
@@ -2784,7 +2835,7 @@
     <mergeCell ref="B17:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Try catch for DQ tracker distance km extraction
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/DriveSummary.xlsx
+++ b/ExcelDriveSummary/DriveSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveAssistant/ExcelDriveSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="382" documentId="13_ncr:1_{E499392B-501C-4B65-8E7E-88D09C8AE449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F150150-1003-49D7-AD76-BA59F40F68D6}"/>
+  <xr:revisionPtr revIDLastSave="425" documentId="13_ncr:1_{E499392B-501C-4B65-8E7E-88D09C8AE449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C809ACC5-E075-4114-A51B-5F09893138F9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="9" r:id="rId1"/>
@@ -802,6 +802,10 @@
     </a>
   </bag>
 </FeaturePropertyBags>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1154,7 +1158,7 @@
   </sheetPr>
   <dimension ref="B2:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -1257,7 +1261,9 @@
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="22">
+        <v>1</v>
+      </c>
       <c r="G6" s="15">
         <v>50</v>
       </c>
@@ -1312,7 +1318,7 @@
       </c>
       <c r="F7" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="G7" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
@@ -1443,7 +1449,7 @@
       </c>
       <c r="F10" s="16">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="16">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
@@ -1552,7 +1558,7 @@
       </c>
       <c r="F13" s="17">
         <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
@@ -1963,7 +1969,7 @@
   <dimension ref="B2:AB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,12 +2066,14 @@
         <v>5</v>
       </c>
       <c r="C6" s="15">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="22">
+        <v>106</v>
+      </c>
       <c r="G6" s="15">
         <v>50</v>
       </c>
@@ -2120,7 +2128,7 @@
       </c>
       <c r="F7" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>3286</v>
       </c>
       <c r="G7" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
@@ -2137,7 +2145,7 @@
         <v>14</v>
       </c>
       <c r="M7" s="31">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
@@ -2175,7 +2183,7 @@
         <v>30</v>
       </c>
       <c r="M8" s="22">
-        <v>300</v>
+        <v>248</v>
       </c>
       <c r="O8" s="1">
         <v>150</v>
@@ -2244,14 +2252,14 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2700</v>
+        <v>2550</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="16">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="G10" s="16">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
@@ -2360,7 +2368,7 @@
       </c>
       <c r="F13" s="17">
         <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
-        <v>1649</v>
+        <v>343</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
@@ -2371,7 +2379,7 @@
       </c>
       <c r="M13" s="1">
         <f ca="1">C10-VLOOKUP(C10,S7:U11,1,TRUE)</f>
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="O13" s="1">
         <v>900</v>
@@ -2455,7 +2463,7 @@
       </c>
       <c r="M16" s="1" t="str">
         <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), "Extract", "Calculate")</f>
-        <v>Extract</v>
+        <v>Calculate</v>
       </c>
       <c r="O16" s="1">
         <v>1350</v>
@@ -2770,7 +2778,7 @@
   </sheetPr>
   <dimension ref="B2:AB50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2867,12 +2875,18 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="15">
+        <v>150</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="22">
+        <v>96</v>
+      </c>
+      <c r="G6" s="15">
+        <v>50</v>
+      </c>
       <c r="I6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2924,11 +2938,11 @@
       </c>
       <c r="F7" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>2976</v>
       </c>
       <c r="G7" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>1550</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2941,7 +2955,7 @@
         <v>14</v>
       </c>
       <c r="M7" s="31">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
@@ -3007,7 +3021,9 @@
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="15">
+        <v>300</v>
+      </c>
       <c r="E9" s="7" t="s">
         <v>17</v>
       </c>
@@ -3046,18 +3062,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2100</v>
+        <v>2550</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="16">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G10" s="16">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>33</v>
@@ -3122,7 +3138,7 @@
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,S7:U11,3,TRUE)</f>
-        <v>Silver</v>
+        <v>Diamond</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="18"/>
@@ -3154,13 +3170,15 @@
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="26">
+        <v>0</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="17" t="str">
+      <c r="F13" s="17">
         <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
-        <v>Unlimited</v>
+        <v>353</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
@@ -3171,7 +3189,7 @@
       </c>
       <c r="M13" s="1">
         <f ca="1">C10-VLOOKUP(C10,S7:U11,1,TRUE)</f>
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="O13" s="1">
         <v>900</v>

</xml_diff>